<commit_message>
Refactor import and export functionality
</commit_message>
<xml_diff>
--- a/wwwroot/files/productReport.xlsx
+++ b/wwwroot/files/productReport.xlsx
@@ -20,7 +20,7 @@
     <t xml:space="preserve">Дата = </t>
   </si>
   <si>
-    <t>02.05.2023</t>
+    <t>04.05.2023</t>
   </si>
   <si>
     <t>ID экспоната</t>
@@ -229,6 +229,7 @@
     <col min="7" max="7" width="16.3083438873291" customWidth="1"/>
     <col min="8" max="8" width="14.772721290588379" customWidth="1"/>
     <col min="9" max="9" width="29.825082778930664" customWidth="1"/>
+    <col min="10" max="10" width="18.32889747619629" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -348,7 +349,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>